<commit_message>
Updated chart example with an example of SLA line plotting
</commit_message>
<xml_diff>
--- a/PercentileChartExample.xlsx
+++ b/PercentileChartExample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="0" windowWidth="18940" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="13400" yWindow="0" windowWidth="18940" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -95,18 +95,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Example Percentile Histogram Graph</t>
   </si>
   <si>
     <t>Uses data imported directly from HdrHistogram's outputPercentileDistribution() for plotting</t>
   </si>
+  <si>
+    <t>Percentile</t>
+  </si>
+  <si>
+    <t>1/(1-P)</t>
+  </si>
+  <si>
+    <t>Require Level</t>
+  </si>
+  <si>
+    <t>Example Stated SLA:</t>
+  </si>
+  <si>
+    <t>Example of derived SLA steps for charting:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -149,7 +167,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -187,11 +205,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -210,6 +265,24 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -228,6 +301,24 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4618,6 +4709,114 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:v>SLA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analysis!$H$44:$H$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.9999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.9999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>999.9999999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>999.9999999999991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000.0000000011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000.0000000011</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000.0000004551</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000.0000004551</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analysis!$I$44:$I$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4626,11 +4825,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2126627128"/>
-        <c:axId val="2122872520"/>
+        <c:axId val="-2063627800"/>
+        <c:axId val="-2063622840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2126627128"/>
+        <c:axId val="-2063627800"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4662,12 +4861,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="2122872520"/>
+        <c:crossAx val="-2063622840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122872520"/>
+        <c:axId val="-2063622840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4715,7 +4914,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126627128"/>
+        <c:crossAx val="-2063627800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5148,25 +5347,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B37:B106"/>
+  <dimension ref="B37:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:9">
       <c r="B37" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="106" ht="30" customHeight="1"/>
+    <row r="41" spans="2:9">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C44">
+        <f>1/(1-B44)</f>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <f>1/(1-G44)</f>
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f>D44</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="C45">
+        <f>1/(1-B45)</f>
+        <v>99.999999999999915</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="G45" s="1">
+        <f>B44</f>
+        <v>0.9</v>
+      </c>
+      <c r="H45">
+        <f>1/(1-G45)</f>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="I45">
+        <f>D44</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="1">
+        <v>0.999</v>
+      </c>
+      <c r="C46">
+        <f>1/(1-B46)</f>
+        <v>999.99999999999909</v>
+      </c>
+      <c r="D46">
+        <v>20</v>
+      </c>
+      <c r="G46" s="1">
+        <f>G45</f>
+        <v>0.9</v>
+      </c>
+      <c r="H46">
+        <f>1/(1-G46)</f>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="I46">
+        <f>D45</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="C47">
+        <f>1/(1-B47)</f>
+        <v>10000.0000000011</v>
+      </c>
+      <c r="D47">
+        <v>100</v>
+      </c>
+      <c r="G47" s="1">
+        <f>B45</f>
+        <v>0.99</v>
+      </c>
+      <c r="H47">
+        <f>1/(1-G47)</f>
+        <v>99.999999999999915</v>
+      </c>
+      <c r="I47">
+        <f>D45</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="1">
+        <v>0.99999000000000005</v>
+      </c>
+      <c r="C48">
+        <f>1/(1-B48)</f>
+        <v>100000.0000004551</v>
+      </c>
+      <c r="D48">
+        <v>100</v>
+      </c>
+      <c r="G48" s="1">
+        <f>G47</f>
+        <v>0.99</v>
+      </c>
+      <c r="H48">
+        <f>1/(1-G48)</f>
+        <v>99.999999999999915</v>
+      </c>
+      <c r="I48">
+        <f>D46</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1000000000000000</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="G49" s="1">
+        <f>B46</f>
+        <v>0.999</v>
+      </c>
+      <c r="H49">
+        <f>1/(1-G49)</f>
+        <v>999.99999999999909</v>
+      </c>
+      <c r="I49">
+        <f>D46</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="1"/>
+      <c r="G50" s="1">
+        <f>G49</f>
+        <v>0.999</v>
+      </c>
+      <c r="H50">
+        <f>1/(1-G50)</f>
+        <v>999.99999999999909</v>
+      </c>
+      <c r="I50">
+        <f>D47</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="1"/>
+      <c r="G51" s="1">
+        <f>B47</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H51">
+        <f>1/(1-G51)</f>
+        <v>10000.0000000011</v>
+      </c>
+      <c r="I51">
+        <f>D47</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="1"/>
+      <c r="G52" s="1">
+        <f>G51</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="H52">
+        <f>1/(1-G52)</f>
+        <v>10000.0000000011</v>
+      </c>
+      <c r="I52">
+        <f>D48</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="1"/>
+      <c r="G53" s="1">
+        <f>B48</f>
+        <v>0.99999000000000005</v>
+      </c>
+      <c r="H53">
+        <f>1/(1-G53)</f>
+        <v>100000.0000004551</v>
+      </c>
+      <c r="I53">
+        <f>D48</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="1"/>
+      <c r="G54" s="1">
+        <f>G53</f>
+        <v>0.99999000000000005</v>
+      </c>
+      <c r="H54">
+        <f>1/(1-G54)</f>
+        <v>100000.0000004551</v>
+      </c>
+      <c r="I54">
+        <f>D49</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="1"/>
+      <c r="G55" s="1">
+        <f>100%</f>
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1000000000000000</v>
+      </c>
+      <c r="I55">
+        <f>D49</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" ht="30" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>